<commit_message>
Added one more word in matrix generator comment
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c09262af37a45c5e/Рабочий стол/Свободная касса/Математик-программист (ANT)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="11_F25DC773A252ABDACC104824A9DE46165ADE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF556C91-7450-4659-A67A-A93DE09EFCCE}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="11_F25DC773A252ABDACC104824A9DE46165ADE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1CE4303-EBA8-4C6B-8D09-9E5B79DF7B42}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -244,7 +244,7 @@
     <t>общее количество символов в барабанах:</t>
   </si>
   <si>
-    <t>СЛУЧАЙНАЯ МАТРИЦА (генерируется заново при любом изменении)</t>
+    <t>СЛУЧАЙНАЯ МАТРИЦА (генерируется заново при любом изменении файла)</t>
   </si>
 </sst>
 </file>
@@ -956,9 +956,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -968,9 +965,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
@@ -1048,6 +1042,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1331,7 +1331,7 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,19 +1394,19 @@
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="40"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="28"/>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="37"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="36"/>
       <c r="S2" s="10" t="s">
         <v>10</v>
       </c>
@@ -1417,24 +1417,24 @@
       <c r="X2" s="30"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="50">
+      <c r="A3" s="48">
         <v>1</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="47">
         <v>8</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="47">
         <v>8</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="47">
         <v>4</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="47">
         <v>7</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="43" t="s">
+      <c r="G3" s="40"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="41" t="s">
         <v>46</v>
       </c>
       <c r="J3" s="33" t="s">
@@ -1458,7 +1458,7 @@
       <c r="P3" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="Q3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="S3" s="13" t="s">
@@ -1479,50 +1479,50 @@
       <c r="X3" s="22"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53">
+      <c r="A4" s="51">
         <v>3</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="50">
         <v>5</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="50">
         <v>5</v>
       </c>
-      <c r="D4" s="52">
+      <c r="D4" s="50">
         <v>6</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="50">
         <v>4</v>
       </c>
-      <c r="G4" s="45"/>
+      <c r="G4" s="43"/>
       <c r="H4" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="46">
+      <c r="I4" s="44">
         <v>8</v>
       </c>
-      <c r="J4" s="47">
+      <c r="J4" s="45">
         <v>7</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="45">
         <v>6</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="45">
         <v>5</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="45">
         <v>4</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="45">
         <v>3</v>
       </c>
-      <c r="O4" s="47">
+      <c r="O4" s="45">
         <v>2</v>
       </c>
-      <c r="P4" s="47">
+      <c r="P4" s="45">
         <v>1</v>
       </c>
-      <c r="Q4" s="48" t="s">
+      <c r="Q4" s="46" t="s">
         <v>5</v>
       </c>
       <c r="S4" s="14" t="s">
@@ -1543,52 +1543,52 @@
       <c r="X4" s="23"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53">
+      <c r="A5" s="51">
         <v>8</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="50">
         <v>1</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="50">
         <v>7</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="50">
         <v>1</v>
       </c>
-      <c r="G5" s="64" t="s">
+      <c r="G5" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="69">
+      <c r="H5" s="67">
         <v>5</v>
       </c>
-      <c r="I5" s="59">
+      <c r="I5" s="57">
         <v>45</v>
       </c>
-      <c r="J5" s="60">
+      <c r="J5" s="58">
         <v>75</v>
       </c>
-      <c r="K5" s="60">
+      <c r="K5" s="58">
         <v>150</v>
       </c>
-      <c r="L5" s="60">
+      <c r="L5" s="58">
         <v>250</v>
       </c>
-      <c r="M5" s="61">
+      <c r="M5" s="59">
         <v>350</v>
       </c>
-      <c r="N5" s="61">
+      <c r="N5" s="59">
         <v>500</v>
       </c>
-      <c r="O5" s="61">
+      <c r="O5" s="59">
         <v>750</v>
       </c>
-      <c r="P5" s="72">
+      <c r="P5" s="70">
         <v>1000</v>
       </c>
-      <c r="Q5" s="70"/>
+      <c r="Q5" s="68"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
@@ -1596,28 +1596,28 @@
       <c r="X5" s="5"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="53">
+      <c r="A6" s="51">
         <v>5</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="50">
         <v>2</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="50">
         <v>6</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="50">
         <v>4</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="50">
         <v>3</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="65">
         <v>5</v>
       </c>
-      <c r="I6" s="62">
+      <c r="I6" s="60">
         <f>(COUNTIF($A$3:$A$84,I$4) + COUNTIF($A$3:$A$84,$Q$4) )*(COUNTIF($B$3:$B$84,I$4) + COUNTIF($B$3:$B$84,$Q$4) )*(COUNTIF($C$3:$C$84,I$4) + COUNTIF($C$3:$C$84,$Q$4) )*(COUNTIF($D$3:$D$84,I$4) + COUNTIF($D$3:$D$84,$Q$4) )*(COUNTIF($E$3:$E$84,I$4) + COUNTIF($E$3:$E$84,$Q$4) )/($H$27*$I$27*$J$27*$K$27*$L$27)</f>
         <v>9.8284928006290231E-5</v>
       </c>
@@ -1645,11 +1645,11 @@
         <f t="shared" si="0"/>
         <v>3.2761642668763415E-5</v>
       </c>
-      <c r="P6" s="73">
+      <c r="P6" s="71">
         <f t="shared" si="0"/>
         <v>3.2761642668763415E-5</v>
       </c>
-      <c r="Q6" s="71"/>
+      <c r="Q6" s="69"/>
       <c r="S6" s="10" t="s">
         <v>17</v>
       </c>
@@ -1660,28 +1660,28 @@
       <c r="X6" s="12"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="53">
+      <c r="A7" s="51">
         <v>6</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="50">
         <v>5</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="50">
         <v>7</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="50">
         <v>8</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="50">
         <v>2</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="67">
+      <c r="H7" s="65">
         <v>5</v>
       </c>
-      <c r="I7" s="62">
+      <c r="I7" s="60">
         <f>I5*I6</f>
         <v>4.42282176028306E-3</v>
       </c>
@@ -1709,11 +1709,11 @@
         <f t="shared" si="1"/>
         <v>2.457123200157256E-2</v>
       </c>
-      <c r="P7" s="73">
+      <c r="P7" s="71">
         <f t="shared" si="1"/>
         <v>3.2761642668763413E-2</v>
       </c>
-      <c r="Q7" s="71"/>
+      <c r="Q7" s="69"/>
       <c r="S7" s="13" t="s">
         <v>13</v>
       </c>
@@ -1732,28 +1732,28 @@
       <c r="X7" s="22"/>
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53">
+      <c r="A8" s="51">
         <v>4</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="50">
         <v>1</v>
       </c>
-      <c r="C8" s="52">
+      <c r="C8" s="50">
         <v>5</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="50">
         <v>3</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="50">
         <v>6</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="67">
+      <c r="H8" s="65">
         <v>4</v>
       </c>
-      <c r="I8" s="62">
+      <c r="I8" s="60">
         <v>15</v>
       </c>
       <c r="J8" s="35">
@@ -1774,10 +1774,10 @@
       <c r="O8" s="34">
         <v>120</v>
       </c>
-      <c r="P8" s="74">
+      <c r="P8" s="72">
         <v>150</v>
       </c>
-      <c r="Q8" s="71"/>
+      <c r="Q8" s="69"/>
       <c r="S8" s="14" t="s">
         <v>21</v>
       </c>
@@ -1796,28 +1796,28 @@
       <c r="X8" s="23"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53">
+      <c r="A9" s="51">
         <v>7</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="50">
         <v>3</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C9" s="50">
         <v>6</v>
       </c>
-      <c r="D9" s="52">
+      <c r="D9" s="50">
         <v>4</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="50">
         <v>8</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="67">
+      <c r="H9" s="65">
         <v>4</v>
       </c>
-      <c r="I9" s="62">
+      <c r="I9" s="60">
         <f>(COUNTIF($A$3:$A$84,I$4) + COUNTIF($A$3:$A$84,$Q$4) )*(COUNTIF($B$3:$B$84,I$4) + COUNTIF($B$3:$B$84,$Q$4) )*(COUNTIF($C$3:$C$84,I$4) + COUNTIF($C$3:$C$84,$Q$4) )*(COUNTIF($D$3:$D$84,I$4) + COUNTIF($D$3:$D$84,$Q$4) )*(COUNTA($E$3:$E$84) - COUNTIF($E$3:$E$84,I$4) - COUNTIF($E$3:$E$84,$Q$4))/($H$27*$I$27*$J$27*$K$27*$L$27)</f>
         <v>3.4399724802201581E-4</v>
       </c>
@@ -1845,11 +1845,11 @@
         <f t="shared" si="2"/>
         <v>1.1466574934067194E-4</v>
       </c>
-      <c r="P9" s="73">
+      <c r="P9" s="71">
         <f t="shared" si="2"/>
         <v>1.1466574934067194E-4</v>
       </c>
-      <c r="Q9" s="71"/>
+      <c r="Q9" s="69"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
@@ -1857,28 +1857,28 @@
       <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="53">
+      <c r="A10" s="51">
         <v>6</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="50">
         <v>4</v>
       </c>
-      <c r="C10" s="52">
+      <c r="C10" s="50">
         <v>8</v>
       </c>
-      <c r="D10" s="52">
+      <c r="D10" s="50">
         <v>2</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="50">
         <v>5</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="67">
+      <c r="H10" s="65">
         <v>4</v>
       </c>
-      <c r="I10" s="62">
+      <c r="I10" s="60">
         <f>I8*I9</f>
         <v>5.1599587203302374E-3</v>
       </c>
@@ -1906,11 +1906,11 @@
         <f t="shared" si="3"/>
         <v>1.3759889920880633E-2</v>
       </c>
-      <c r="P10" s="73">
+      <c r="P10" s="71">
         <f t="shared" si="3"/>
         <v>1.7199862401100791E-2</v>
       </c>
-      <c r="Q10" s="71"/>
+      <c r="Q10" s="69"/>
       <c r="S10" s="10" t="s">
         <v>18</v>
       </c>
@@ -1921,28 +1921,28 @@
       <c r="X10" s="12"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
+      <c r="A11" s="51">
         <v>4</v>
       </c>
-      <c r="B11" s="52">
+      <c r="B11" s="50">
         <v>5</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="50">
         <v>2</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D11" s="50">
         <v>5</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="67">
+      <c r="H11" s="65">
         <v>3</v>
       </c>
-      <c r="I11" s="62">
+      <c r="I11" s="60">
         <v>3</v>
       </c>
       <c r="J11" s="35">
@@ -1963,10 +1963,10 @@
       <c r="O11" s="34">
         <v>20</v>
       </c>
-      <c r="P11" s="74">
+      <c r="P11" s="72">
         <v>30</v>
       </c>
-      <c r="Q11" s="71"/>
+      <c r="Q11" s="69"/>
       <c r="S11" s="13" t="s">
         <v>13</v>
       </c>
@@ -1985,26 +1985,26 @@
       <c r="X11" s="22"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53">
+      <c r="A12" s="51">
         <v>2</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="50">
         <v>6</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C12" s="50">
         <v>4</v>
       </c>
-      <c r="D12" s="52">
+      <c r="D12" s="50">
         <v>7</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="G12" s="65" t="s">
+      <c r="E12" s="50"/>
+      <c r="G12" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="67">
+      <c r="H12" s="65">
         <v>3</v>
       </c>
-      <c r="I12" s="62">
+      <c r="I12" s="60">
         <f>(COUNTIF($A$3:$A$84,I$4) + COUNTIF($A$3:$A$84,$Q$4) )*(COUNTIF($B$3:$B$84,I$4) + COUNTIF($B$3:$B$84,$Q$4) )*(COUNTIF($C$3:$C$84,I$4) + COUNTIF($C$3:$C$84,$Q$4) )*(COUNTA($D$3:$D$84) - COUNTIF($D$3:$D$84,I$4) - COUNTIF($D$3:$D$84,$Q$4) )*(COUNTA($E$3:$E$84) - COUNTIF($E$3:$E$84,I$4) - COUNTIF($E$3:$E$84,$Q$4))/($H$27*$I$27*$J$27*$K$27*$L$27)</f>
         <v>2.0639834881320948E-3</v>
       </c>
@@ -2032,11 +2032,11 @@
         <f t="shared" si="4"/>
         <v>6.8799449604403163E-4</v>
       </c>
-      <c r="P12" s="73">
+      <c r="P12" s="71">
         <f t="shared" si="4"/>
         <v>6.8799449604403163E-4</v>
       </c>
-      <c r="Q12" s="71"/>
+      <c r="Q12" s="69"/>
       <c r="S12" s="14" t="s">
         <v>24</v>
       </c>
@@ -2055,54 +2055,54 @@
       <c r="X12" s="23"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="53">
+      <c r="A13" s="51">
         <v>8</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="50">
         <v>4</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C13" s="50">
         <v>3</v>
       </c>
-      <c r="D13" s="52">
+      <c r="D13" s="50">
         <v>1</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="G13" s="65" t="s">
+      <c r="E13" s="51"/>
+      <c r="G13" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="68">
+      <c r="H13" s="66">
         <v>3</v>
       </c>
-      <c r="I13" s="63">
+      <c r="I13" s="61">
         <f>I11*I12</f>
         <v>6.1919504643962843E-3</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="38">
         <f t="shared" ref="J13:P13" si="5">J11*J12</f>
         <v>6.4499484004127972E-3</v>
       </c>
-      <c r="K13" s="39">
+      <c r="K13" s="38">
         <f t="shared" si="5"/>
         <v>3.8527691778465774E-2</v>
       </c>
-      <c r="L13" s="39">
+      <c r="L13" s="38">
         <f t="shared" si="5"/>
         <v>3.5474716202270384E-2</v>
       </c>
-      <c r="M13" s="39">
+      <c r="M13" s="38">
         <f t="shared" si="5"/>
         <v>4.1279669762641899E-2</v>
       </c>
-      <c r="N13" s="39">
+      <c r="N13" s="38">
         <f t="shared" si="5"/>
         <v>3.0959752321981421E-2</v>
       </c>
-      <c r="O13" s="39">
+      <c r="O13" s="38">
         <f t="shared" si="5"/>
         <v>1.3759889920880633E-2</v>
       </c>
-      <c r="P13" s="75">
+      <c r="P13" s="73">
         <f t="shared" si="5"/>
         <v>2.063983488132095E-2</v>
       </c>
@@ -2114,19 +2114,19 @@
       <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="53">
+      <c r="A14" s="51">
         <v>4</v>
       </c>
-      <c r="B14" s="52">
+      <c r="B14" s="50">
         <v>7</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="52">
+      <c r="D14" s="50">
         <v>5</v>
       </c>
-      <c r="E14" s="53"/>
+      <c r="E14" s="51"/>
       <c r="S14" s="10" t="s">
         <v>19</v>
       </c>
@@ -2137,17 +2137,17 @@
       <c r="X14" s="12"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52">
+      <c r="A15" s="50"/>
+      <c r="B15" s="50">
         <v>6</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C15" s="50">
         <v>5</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="53"/>
+      <c r="E15" s="51"/>
       <c r="S15" s="13" t="s">
         <v>13</v>
       </c>
@@ -2166,17 +2166,17 @@
       <c r="X15" s="22"/>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50">
         <v>4</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="50">
         <v>6</v>
       </c>
-      <c r="D16" s="52">
+      <c r="D16" s="50">
         <v>7</v>
       </c>
-      <c r="E16" s="53"/>
+      <c r="E16" s="51"/>
       <c r="G16" s="7" t="s">
         <v>7</v>
       </c>
@@ -2199,15 +2199,15 @@
       <c r="X16" s="23"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50">
         <v>3</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C17" s="50">
         <v>3</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
       <c r="G17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2216,15 +2216,15 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52">
+      <c r="A18" s="50"/>
+      <c r="B18" s="50">
         <v>6</v>
       </c>
-      <c r="C18" s="52">
+      <c r="C18" s="50">
         <v>5</v>
       </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
       <c r="G18" s="2" t="str">
         <f>SUM(I7:P7,I10:P10,I13:P13) / 1 * 100 &amp; "%"</f>
         <v>86,5060936655364%</v>
@@ -2243,15 +2243,15 @@
       <c r="X18" s="12"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52">
+      <c r="A19" s="50"/>
+      <c r="B19" s="50">
         <v>7</v>
       </c>
-      <c r="C19" s="52">
+      <c r="C19" s="50">
         <v>7</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
       <c r="S19" s="13" t="s">
         <v>13</v>
       </c>
@@ -2270,13 +2270,13 @@
       <c r="X19" s="22"/>
     </row>
     <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52">
+      <c r="A20" s="50"/>
+      <c r="B20" s="50">
         <v>5</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="53"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
       <c r="S20" s="14" t="s">
         <v>30</v>
       </c>
@@ -2295,185 +2295,185 @@
       <c r="X20" s="23"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52">
+      <c r="A21" s="50"/>
+      <c r="B21" s="50">
         <v>3</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
       <c r="H21" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="53"/>
-      <c r="H22" s="79" cm="1">
+      <c r="A22" s="52"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="H22" s="77" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">INDEX(A$3:A$85,MOD(H$26, H$27)+1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="I22" s="79" cm="1">
+        <v>3</v>
+      </c>
+      <c r="I22" s="77" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">INDEX(B$3:B$85,MOD(I$26, I$27)+1,1)</f>
         <v>6</v>
       </c>
-      <c r="J22" s="79" cm="1">
+      <c r="J22" s="77" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">INDEX(C$3:C$85,MOD(J$26, J$27)+1,1)</f>
         <v>5</v>
       </c>
-      <c r="K22" s="79" cm="1">
+      <c r="K22" s="77" cm="1">
         <f t="array" aca="1" ref="K22" ca="1">INDEX(D$3:D$85,MOD(K$26, K$27)+1,1)</f>
+        <v>5</v>
+      </c>
+      <c r="L22" s="79" cm="1">
+        <f t="array" aca="1" ref="L22" ca="1">INDEX(E$3:E$85,MOD(L$26, L$27)+1,1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="52"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="H23" s="77" cm="1">
+        <f t="array" aca="1" ref="H23" ca="1">INDEX(A$3:A$85,MOD(H$26 + 1, H$27)+1,1)</f>
+        <v>8</v>
+      </c>
+      <c r="I23" s="77" cm="1">
+        <f t="array" aca="1" ref="I23" ca="1">INDEX(B$3:B$85,MOD(I$26 + 1, I$27)+1,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J23" s="77" cm="1">
+        <f t="array" aca="1" ref="J23" ca="1">INDEX(C$3:C$85,MOD(J$26 + 1, J$27)+1,1)</f>
         <v>7</v>
       </c>
-      <c r="L22" s="81" cm="1">
-        <f t="array" aca="1" ref="L22" ca="1">INDEX(E$3:E$85,MOD(L$26, L$27)+1,1)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="H23" s="79" cm="1">
-        <f t="array" aca="1" ref="H23" ca="1">INDEX(A$3:A$85,MOD(H$26 + 1, H$27)+1,1)</f>
-        <v>3</v>
-      </c>
-      <c r="I23" s="79" cm="1">
-        <f t="array" aca="1" ref="I23" ca="1">INDEX(B$3:B$85,MOD(I$26 + 1, I$27)+1,1)</f>
+      <c r="K23" s="77" cm="1">
+        <f t="array" aca="1" ref="K23" ca="1">INDEX(D$3:D$85,MOD(K$26 + 1, K$27)+1,1)</f>
         <v>7</v>
       </c>
-      <c r="J23" s="79" cm="1">
-        <f t="array" aca="1" ref="J23" ca="1">INDEX(C$3:C$85,MOD(J$26 + 1, J$27)+1,1)</f>
-        <v>6</v>
-      </c>
-      <c r="K23" s="79" cm="1">
-        <f t="array" aca="1" ref="K23" ca="1">INDEX(D$3:D$85,MOD(K$26 + 1, K$27)+1,1)</f>
-        <v>4</v>
-      </c>
-      <c r="L23" s="81" cm="1">
+      <c r="L23" s="79" cm="1">
         <f t="array" aca="1" ref="L23" ca="1">INDEX(E$3:E$85,MOD(L$26 + 1, L$27)+1,1)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
-      <c r="H24" s="82" cm="1">
+      <c r="A24" s="52"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
+      <c r="H24" s="80" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">INDEX(A$3:A$85,MOD(H$26 + 2, H$27)+1,1)</f>
+        <v>5</v>
+      </c>
+      <c r="I24" s="80" cm="1">
+        <f t="array" aca="1" ref="I24" ca="1">INDEX(B$3:B$85,MOD(I$26 + 2, I$27)+1,1)</f>
+        <v>7</v>
+      </c>
+      <c r="J24" s="80" cm="1">
+        <f t="array" aca="1" ref="J24" ca="1">INDEX(C$3:C$85,MOD(J$26 + 2, J$27)+1,1)</f>
         <v>8</v>
       </c>
-      <c r="I24" s="82" cm="1">
-        <f t="array" aca="1" ref="I24" ca="1">INDEX(B$3:B$85,MOD(I$26 + 2, I$27)+1,1)</f>
+      <c r="K24" s="80" cm="1">
+        <f t="array" aca="1" ref="K24" ca="1">INDEX(D$3:D$85,MOD(K$26 + 2, K$27)+1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="81" cm="1">
+        <f t="array" aca="1" ref="L24" ca="1">INDEX(E$3:E$85,MOD(L$26 + 2, L$27)+1,1)</f>
         <v>5</v>
       </c>
-      <c r="J24" s="82" cm="1">
-        <f t="array" aca="1" ref="J24" ca="1">INDEX(C$3:C$85,MOD(J$26 + 2, J$27)+1,1)</f>
-        <v>3</v>
-      </c>
-      <c r="K24" s="82" cm="1">
-        <f t="array" aca="1" ref="K24" ca="1">INDEX(D$3:D$85,MOD(K$26 + 2, K$27)+1,1)</f>
+    </row>
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="52"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+    </row>
+    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="52"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="51"/>
+      <c r="G26" s="78" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="74">
+        <f ca="1">RANDBETWEEN(1,COUNTA(A$3:A$85))</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="75">
+        <f t="shared" ref="I26:L26" ca="1" si="6">RANDBETWEEN(1,COUNTA(B$3:B$85))</f>
+        <v>9</v>
+      </c>
+      <c r="J26" s="75">
+        <f t="shared" ca="1" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="K26" s="75">
+        <f t="shared" ca="1" si="6"/>
         <v>8</v>
       </c>
-      <c r="L24" s="83" cm="1">
-        <f t="array" aca="1" ref="L24" ca="1">INDEX(E$3:E$85,MOD(L$26 + 2, L$27)+1,1)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-    </row>
-    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="53"/>
-      <c r="G26" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="H26" s="76">
-        <f ca="1">RANDBETWEEN(1,COUNTA(A$3:A$85))</f>
-        <v>12</v>
-      </c>
-      <c r="I26" s="77">
-        <f t="shared" ref="I26:L26" ca="1" si="6">RANDBETWEEN(1,COUNTA(B$3:B$85))</f>
-        <v>15</v>
-      </c>
-      <c r="J26" s="77">
+      <c r="L26" s="76">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
-      </c>
-      <c r="K26" s="77">
-        <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L26" s="78">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="51"/>
-      <c r="G27" s="80" t="s">
+      <c r="A27" s="52"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="49"/>
+      <c r="G27" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="H27" s="84">
+      <c r="H27" s="82">
         <f>COUNTA(A$3:A$85)</f>
         <v>12</v>
       </c>
-      <c r="I27" s="85">
+      <c r="I27" s="83">
         <f t="shared" ref="I27:L27" si="7">COUNTA(B$3:B$85)</f>
         <v>19</v>
       </c>
-      <c r="J27" s="85">
+      <c r="J27" s="83">
         <f t="shared" si="7"/>
         <v>17</v>
       </c>
-      <c r="K27" s="85">
+      <c r="K27" s="83">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="L27" s="66">
+      <c r="L27" s="64">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="53"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="51"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="51"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="53"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="51"/>
       <c r="G30" s="31"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2483,11 +2483,11 @@
       <c r="P30" s="1"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="51"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -2496,11 +2496,11 @@
       <c r="P31" s="5"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="53"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="51"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -2509,11 +2509,11 @@
       <c r="P32" s="5"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="53"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="51"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -2522,11 +2522,11 @@
       <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="53"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="51"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -2535,11 +2535,11 @@
       <c r="P34" s="5"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="51"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -2548,11 +2548,11 @@
       <c r="P35" s="5"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="53"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="51"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -2561,11 +2561,11 @@
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="51"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -2574,11 +2574,11 @@
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="53"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="51"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
@@ -2587,63 +2587,63 @@
       <c r="P38" s="5"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="51"/>
       <c r="P39" s="5"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="51"/>
       <c r="P40" s="5"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
-      <c r="B41" s="52"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="51"/>
       <c r="P41" s="5"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="53"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="51"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="53"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="51"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
-      <c r="B44" s="52"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="53"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="51"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="51"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="55"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="58"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>